<commit_message>
[ENote] Add Spring MVC dependency + NoteController
</commit_message>
<xml_diff>
--- a/data/api.xlsx
+++ b/data/api.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -155,10 +155,10 @@
     <t>Удалить конкрутную метку конкретной заметки конкретного блокнота</t>
   </si>
   <si>
-    <t>notes/search_title</t>
-  </si>
-  <si>
-    <t>notes/search_label</t>
+    <t>notes/search_title/{title}</t>
+  </si>
+  <si>
+    <t>notes/search_label/{label}</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
[ENote] Configure Spring MVC and Swagger
</commit_message>
<xml_diff>
--- a/data/api.xlsx
+++ b/data/api.xlsx
@@ -155,10 +155,10 @@
     <t>Удалить конкрутную метку конкретной заметки конкретного блокнота</t>
   </si>
   <si>
-    <t>notes/search_title/{title}</t>
-  </si>
-  <si>
-    <t>notes/search_label/{label}</t>
+    <t>notes/search_title</t>
+  </si>
+  <si>
+    <t>notes/search_label</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -566,7 +566,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -577,7 +577,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
[ENote] Small change in api map
</commit_message>
<xml_diff>
--- a/data/api.xlsx
+++ b/data/api.xlsx
@@ -155,10 +155,10 @@
     <t>Удалить конкрутную метку конкретной заметки конкретного блокнота</t>
   </si>
   <si>
-    <t>notes/search_title/{title}</t>
-  </si>
-  <si>
-    <t>notes/search_label/{label}</t>
+    <t>notes/search_title</t>
+  </si>
+  <si>
+    <t>notes/search_label</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -566,7 +566,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -577,7 +577,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
[ENote] Add small change in api map + remove MVC & controller
</commit_message>
<xml_diff>
--- a/data/api.xlsx
+++ b/data/api.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -566,7 +566,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -577,7 +577,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>

</xml_diff>